<commit_message>
ontology metadata for default/OWL; contributors
</commit_message>
<xml_diff>
--- a/code/vocab_csv/purpose_processing.xlsx
+++ b/code/vocab_csv/purpose_processing.xlsx
@@ -15313,8 +15313,10 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1.0" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection activeCell="C2" sqref="C2" pane="topRight"/>
+      <pane xSplit="1.0" ySplit="1.0" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1" pane="topRight"/>
+      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
+      <selection activeCell="B2" sqref="B2" pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
@@ -17483,13 +17485,13 @@
       <c r="K52" s="45">
         <v>43592.0</v>
       </c>
-      <c r="L52" s="45"/>
+      <c r="L52" s="45">
+        <v>44848.0</v>
+      </c>
       <c r="M52" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="N52" s="45">
-        <v>44848.0</v>
-      </c>
+      <c r="N52" s="20"/>
       <c r="O52" s="46" t="s">
         <v>451</v>
       </c>

</xml_diff>